<commit_message>
mapeado até o nó 42 e ajustado nimeros das latitudes e longitudes
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota_2/Ativos_Russas.xlsx
+++ b/Algoritmo_Rota_2/Ativos_Russas.xlsx
@@ -458,23 +458,23 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>27, 11, 10, 2, 25</t>
+          <t>9, 19, 31, 4, 11</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>27 -&gt; 27 -&gt; 25 -&gt; 2 -&gt; 10 -&gt; 11 -&gt; 27</t>
+          <t>29 -&gt; 31 -&gt; 31 -&gt; 19 -&gt; 19 -&gt; 11 -&gt; 11 -&gt; 4 -&gt; 4 -&gt; 9</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.1214172840118408</v>
       </c>
     </row>
     <row r="3">
@@ -482,23 +482,23 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>17, 31, 22, 6, 8</t>
+          <t>10, 19, 8, 26, 13</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27 -&gt; 31 -&gt; 17 -&gt; 22 -&gt; 8 -&gt; 6 -&gt; 27</t>
+          <t>9 -&gt; 13 -&gt; 13 -&gt; 19 -&gt; 19 -&gt; 10 -&gt; 10 -&gt; 8 -&gt; 8 -&gt; 26</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1528</v>
+        <v>1172</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.1215567588806152</v>
       </c>
     </row>
     <row r="4">
@@ -506,23 +506,23 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24, 21, 6, 15, 26</t>
+          <t>6, 30, 21, 10, 4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31 -&gt; 24 -&gt; 21 -&gt; 15 -&gt; 6 -&gt; 26 -&gt; 31</t>
+          <t>25 -&gt; 6 -&gt; 6 -&gt; 4 -&gt; 4 -&gt; 10 -&gt; 10 -&gt; 21 -&gt; 21 -&gt; 30</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1534</v>
+        <v>1163</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.1183443069458008</v>
       </c>
     </row>
     <row r="5">
@@ -530,23 +530,23 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>22, 19, 11, 21, 12</t>
+          <t>18, 24, 2, 8, 28</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13 -&gt; 12 -&gt; 11 -&gt; 22 -&gt; 21 -&gt; 19 -&gt; 13</t>
+          <t>5 -&gt; 2 -&gt; 2 -&gt; 8 -&gt; 8 -&gt; 28 -&gt; 28 -&gt; 24 -&gt; 24 -&gt; 18</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>954</v>
+        <v>1196</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.1190147399902344</v>
       </c>
     </row>
     <row r="6">
@@ -554,23 +554,23 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>28, 4, 18, 30, 10</t>
+          <t>4, 17, 11, 18, 8</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15 -&gt; 18 -&gt; 10 -&gt; 4 -&gt; 28 -&gt; 30 -&gt; 15</t>
+          <t>8 -&gt; 8 -&gt; 8 -&gt; 4 -&gt; 4 -&gt; 11 -&gt; 11 -&gt; 18 -&gt; 18 -&gt; 17</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1228</v>
+        <v>869</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.09990334510803223</v>
       </c>
     </row>
     <row r="7">
@@ -578,23 +578,23 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>16, 20, 8, 14, 12</t>
+          <t>3, 4, 12, 23, 1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5 -&gt; 14 -&gt; 20 -&gt; 16 -&gt; 12 -&gt; 8 -&gt; 5</t>
+          <t>21 -&gt; 23 -&gt; 23 -&gt; 12 -&gt; 12 -&gt; 4 -&gt; 4 -&gt; 3 -&gt; 3 -&gt; 1</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1072</v>
+        <v>1435</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.1154119968414307</v>
       </c>
     </row>
     <row r="8">
@@ -602,23 +602,23 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2, 25, 1, 9, 11</t>
+          <t>11, 15, 6, 25, 9</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14 -&gt; 11 -&gt; 9 -&gt; 25 -&gt; 1 -&gt; 2 -&gt; 14</t>
+          <t>25 -&gt; 25 -&gt; 25 -&gt; 6 -&gt; 6 -&gt; 9 -&gt; 9 -&gt; 11 -&gt; 11 -&gt; 15</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1537</v>
+        <v>614</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.1045219898223877</v>
       </c>
     </row>
     <row r="9">
@@ -626,23 +626,23 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6, 14, 3, 26, 17</t>
+          <t>3, 30, 21, 7, 14</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>18 -&gt; 14 -&gt; 17 -&gt; 26 -&gt; 3 -&gt; 6 -&gt; 18</t>
+          <t>6 -&gt; 3 -&gt; 3 -&gt; 30 -&gt; 30 -&gt; 7 -&gt; 7 -&gt; 14 -&gt; 14 -&gt; 21</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1379</v>
+        <v>1125</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.1311888694763184</v>
       </c>
     </row>
     <row r="10">
@@ -650,23 +650,23 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4, 14, 17, 3, 13</t>
+          <t>19, 10, 25, 26, 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7 -&gt; 4 -&gt; 3 -&gt; 13 -&gt; 17 -&gt; 14 -&gt; 7</t>
+          <t>19 -&gt; 19 -&gt; 19 -&gt; 10 -&gt; 10 -&gt; 9 -&gt; 9 -&gt; 26 -&gt; 26 -&gt; 25</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1089</v>
+        <v>848</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.1345524787902832</v>
       </c>
     </row>
     <row r="11">
@@ -674,23 +674,23 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>25, 19, 10, 11, 15</t>
+          <t>31, 9, 22, 28, 19</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>22 -&gt; 15 -&gt; 10 -&gt; 11 -&gt; 25 -&gt; 19 -&gt; 22</t>
+          <t>13 -&gt; 9 -&gt; 9 -&gt; 28 -&gt; 28 -&gt; 31 -&gt; 31 -&gt; 19 -&gt; 19 -&gt; 22</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1642</v>
+        <v>836</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.1235864162445068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>